<commit_message>
Update Calculator excel with new feautre
</commit_message>
<xml_diff>
--- a/Calcolautor excel.xlsx
+++ b/Calcolautor excel.xlsx
@@ -429,7 +429,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -748,6 +748,30 @@
         <f>B4^2</f>
         <v>16</v>
       </c>
+      <c r="F13">
+        <f>(B1+B2)^2</f>
+        <v>9</v>
+      </c>
+      <c r="G13">
+        <f>(B1+B3)^2</f>
+        <v>16</v>
+      </c>
+      <c r="H13">
+        <f>(B1+B4)^2</f>
+        <v>25</v>
+      </c>
+      <c r="I13">
+        <f>(B2+B3)^2</f>
+        <v>25</v>
+      </c>
+      <c r="J13">
+        <f>(B2+B4)^2</f>
+        <v>36</v>
+      </c>
+      <c r="K13">
+        <f>(B3+B4)^2</f>
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
@@ -769,6 +793,30 @@
         <f>B4^3</f>
         <v>64</v>
       </c>
+      <c r="F14">
+        <f>(B1+B2)^3</f>
+        <v>27</v>
+      </c>
+      <c r="G14">
+        <f>(B1+B3)^3</f>
+        <v>64</v>
+      </c>
+      <c r="H14">
+        <f>(B1+B4)^3</f>
+        <v>125</v>
+      </c>
+      <c r="I14">
+        <f>(B2+B3)^3</f>
+        <v>125</v>
+      </c>
+      <c r="J14">
+        <f>(B2+B4)^3</f>
+        <v>216</v>
+      </c>
+      <c r="K14">
+        <f>(B3+B4)^3</f>
+        <v>343</v>
+      </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2" t="s">
@@ -789,6 +837,30 @@
       <c r="E15">
         <f>SQRT(B4)</f>
         <v>2</v>
+      </c>
+      <c r="F15">
+        <f>SQRT(B1+B2)</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="G15">
+        <f>SQRT(B1+B3)</f>
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <f>SQRT(B1+B4)</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="I15">
+        <f>SQRT(B2+B3)</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="J15">
+        <f>SQRT(B2+B4)</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="K15">
+        <f>SQRT(B3+B4)</f>
+        <v>2.6457513110645907</v>
       </c>
     </row>
   </sheetData>

</xml_diff>